<commit_message>
Updated fast rendererers chart (Y axis start with 0)
</commit_message>
<xml_diff>
--- a/src/Fast Renderers/FastRenderers Performance.xlsx
+++ b/src/Fast Renderers/FastRenderers Performance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\GitHub\xamarin-forms-perf-playground\src\Fast Renderers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADC1F4C-31FE-497A-B80B-FB92B01EA2B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B042D99B-A61F-4D39-B922-F535186A5C61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,6 +444,7 @@
         <c:axId val="235177488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1365,7 +1366,7 @@
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>